<commit_message>
comleted validating Santa toy
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorji/Documents/GitHub/Comp3522/assignment-2---the-supply-chain-nash-and-taylor_assign2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A448FFDA-028D-8543-9304-3260498FEF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE2742F-E314-6A4B-B71F-18DE4A495FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Sea Salt</t>
+  </si>
+  <si>
+    <t>GJ</t>
   </si>
 </sst>
 </file>
@@ -667,9 +670,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24:C24"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -791,7 +794,7 @@
         <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="I2">
         <v>5</v>

</xml_diff>

<commit_message>
commit for dev merging
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorji/Documents/GitHub/Comp3522/assignment-2---the-supply-chain-nash-and-taylor_assign2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA69DC2-189B-2B42-82AA-2193AF134FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE3389D-FE30-5D49-AA5E-10E1552783B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -667,9 +667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="173" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q16" sqref="Q16"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
commit for merging dev
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorji/Documents/GitHub/Comp3522/assignment-2---the-supply-chain-nash-and-taylor_assign2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE3389D-FE30-5D49-AA5E-10E1552783B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB94546-EDCE-074D-9311-37386572DF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="28800" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Sea Salt</t>
+  </si>
+  <si>
+    <t>Mr. Hoppers_2</t>
   </si>
 </sst>
 </file>
@@ -665,11 +668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1264,14 +1267,148 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="1"/>
+    <row r="16" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>30</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>30</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>